<commit_message>
add context to final report
</commit_message>
<xml_diff>
--- a/input/source_B.xlsx
+++ b/input/source_B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anaken Codes\github\data-tools-datasets-differentials\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FE0F05-467B-433A-B771-FBD1AA830A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A58C16-F693-4C38-9D3C-4678F0B76008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,7 +426,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -437,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -470,7 +470,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -481,7 +481,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -492,7 +492,7 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
highlight in report the changed cells i.e. diffferential values
</commit_message>
<xml_diff>
--- a/input/source_B.xlsx
+++ b/input/source_B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anaken Codes\github\data-tools-datasets-differentials\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A58C16-F693-4C38-9D3C-4678F0B76008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B67BDE-2E2A-4048-B331-8CA2D003FCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Malaysia</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Revenue for Feb 2022 ($ 'mil)</t>
+  </si>
+  <si>
+    <t>North Americas</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,7 +404,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>101</v>
@@ -464,10 +464,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
       </c>
       <c r="C7">
         <v>71</v>
@@ -475,10 +475,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>66</v>
@@ -486,10 +486,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
       <c r="C9">
         <v>3</v>

</xml_diff>